<commit_message>
Moved statistical datasets and results
</commit_message>
<xml_diff>
--- a/7. Statistic Analysis/Results/Java/Correctness/Wilcoxon - correct.xlsx
+++ b/7. Statistic Analysis/Results/Java/Correctness/Wilcoxon - correct.xlsx
@@ -14,7 +14,53 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t xml:space="preserve"><![CDATA[Valid]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[T]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[Z]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[p-value]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[NbUnique Operands & EffortTo Implement]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[NbOperands & EffortTo Implement]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[NbUnique Operators & EffortTo Implement]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[Program Length & EffortTo Implement]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[Difficulty Level & Difficulty Level]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[Program Level & Program Level]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[EffortTo Implement & NbOperands]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[EffortTo Implement & NbUnique Operators]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[EffortTo Implement & Program Length]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[EffortTo Implement & EffortTo Implement]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[TimeTo Implement & TimeTo Implement]]></t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -343,169 +389,217 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.596372" customWidth="1"/>
-    <col min="2" max="2" width="9.593605" customWidth="1"/>
+    <col min="1" max="1" width="56.949888" customWidth="1"/>
+    <col min="2" max="2" width="6.596372" customWidth="1"/>
     <col min="3" max="3" width="9.593605" customWidth="1"/>
     <col min="4" max="4" width="9.593605" customWidth="1"/>
+    <col min="5" max="5" width="9.593605" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="n" s="0">
+      <c r="B1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B2" t="n" s="0">
         <v>198</v>
       </c>
-      <c r="B1" t="n" s="0">
+      <c r="C2" t="n" s="0">
         <v>8382.500000</v>
       </c>
-      <c r="C1" t="n" s="0">
+      <c r="D2" t="n" s="0">
         <v>1.818349</v>
       </c>
-      <c r="D1" t="n" s="0">
+      <c r="E2" t="n" s="0">
         <v>0.069012</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n" s="0">
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B3" t="n" s="0">
         <v>198</v>
       </c>
-      <c r="B2" t="n" s="0">
+      <c r="C3" t="n" s="0">
         <v>8270.000000</v>
       </c>
-      <c r="C2" t="n" s="0">
+      <c r="D3" t="n" s="0">
         <v>1.957698</v>
       </c>
-      <c r="D2" t="n" s="0">
+      <c r="E3" t="n" s="0">
         <v>0.050266</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n" s="0">
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B4" t="n" s="0">
         <v>198</v>
       </c>
-      <c r="B3" t="n" s="0">
+      <c r="C4" t="n" s="0">
         <v>9366.000000</v>
       </c>
-      <c r="C3" t="n" s="0">
+      <c r="D4" t="n" s="0">
         <v>0.600130</v>
       </c>
-      <c r="D3" t="n" s="0">
+      <c r="E4" t="n" s="0">
         <v>0.548420</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n" s="0">
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B5" t="n" s="0">
         <v>198</v>
       </c>
-      <c r="B4" t="n" s="0">
+      <c r="C5" t="n" s="0">
         <v>9849.000000</v>
       </c>
-      <c r="C4" t="n" s="0">
+      <c r="D5" t="n" s="0">
         <v>0.001858</v>
       </c>
-      <c r="D4" t="n" s="0">
+      <c r="E5" t="n" s="0">
         <v>0.998518</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n" s="0">
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B6" t="n" s="0">
         <v>15</v>
       </c>
-      <c r="B5" t="n" s="0">
+      <c r="C6" t="n" s="0">
         <v>34.000000</v>
       </c>
-      <c r="C5" t="n" s="0">
+      <c r="D6" t="n" s="0">
         <v>1.476701</v>
       </c>
-      <c r="D5" t="n" s="0">
+      <c r="E6" t="n" s="0">
         <v>0.139757</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n" s="0">
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B7" t="n" s="0">
         <v>14</v>
       </c>
-      <c r="B6" t="n" s="0">
+      <c r="C7" t="n" s="0">
         <v>41.000000</v>
       </c>
-      <c r="C6" t="n" s="0">
+      <c r="D7" t="n" s="0">
         <v>0.721930</v>
       </c>
-      <c r="D6" t="n" s="0">
+      <c r="E7" t="n" s="0">
         <v>0.470338</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n" s="0">
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B8" t="n" s="0">
         <v>198</v>
       </c>
-      <c r="B7" t="n" s="0">
+      <c r="C8" t="n" s="0">
         <v>8413.000000</v>
       </c>
-      <c r="C7" t="n" s="0">
+      <c r="D8" t="n" s="0">
         <v>1.780570</v>
       </c>
-      <c r="D7" t="n" s="0">
+      <c r="E8" t="n" s="0">
         <v>0.074984</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n" s="0">
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B9" t="n" s="0">
         <v>198</v>
       </c>
-      <c r="B8" t="n" s="0">
+      <c r="C9" t="n" s="0">
         <v>9109.000000</v>
       </c>
-      <c r="C8" t="n" s="0">
+      <c r="D9" t="n" s="0">
         <v>0.918465</v>
       </c>
-      <c r="D8" t="n" s="0">
+      <c r="E9" t="n" s="0">
         <v>0.358376</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n" s="0">
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B10" t="n" s="0">
         <v>198</v>
       </c>
-      <c r="B9" t="n" s="0">
+      <c r="C10" t="n" s="0">
         <v>9614.000000</v>
       </c>
-      <c r="C9" t="n" s="0">
+      <c r="D10" t="n" s="0">
         <v>0.292942</v>
       </c>
-      <c r="D9" t="n" s="0">
+      <c r="E10" t="n" s="0">
         <v>0.769566</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="n" s="0">
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B11" t="n" s="0">
         <v>16</v>
       </c>
-      <c r="B10" t="n" s="0">
+      <c r="C11" t="n" s="0">
         <v>40.000000</v>
       </c>
-      <c r="C10" t="n" s="0">
+      <c r="D11" t="n" s="0">
         <v>1.447846</v>
       </c>
-      <c r="D10" t="n" s="0">
+      <c r="E11" t="n" s="0">
         <v>0.147661</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="n" s="0">
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B12" t="n" s="0">
         <v>15</v>
       </c>
-      <c r="B11" t="n" s="0">
+      <c r="C12" t="n" s="0">
         <v>39.000000</v>
       </c>
-      <c r="C11" t="n" s="0">
+      <c r="D12" t="n" s="0">
         <v>1.192720</v>
       </c>
-      <c r="D11" t="n" s="0">
+      <c r="E12" t="n" s="0">
         <v>0.232980</v>
       </c>
     </row>

</xml_diff>